<commit_message>
Add .venv to .gitignore
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,20 +446,15 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>student_birthdate</t>
+          <t>event_name</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>student_age</t>
+          <t>result_month</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>event_name</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>event_result</t>
         </is>
@@ -478,18 +473,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2010-04-30</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>14</v>
-      </c>
+          <t>Разметка данных на CVAT для начинающих</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
-        <is>
-          <t>Разметка данных на CVAT для начинающих</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
         <is>
           <t>Сертификат участника</t>
         </is>
@@ -508,18 +496,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2011-05-11</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>13</v>
-      </c>
+          <t>Разметка данных на CVAT для начинающих</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
-        <is>
-          <t>Разметка данных на CVAT для начинающих</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
         <is>
           <t>Сертификат участника</t>
         </is>
@@ -538,18 +519,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2013-10-21</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>11</v>
-      </c>
+          <t>Разметка данных на CVAT для начинающих</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
-        <is>
-          <t>Разметка данных на CVAT для начинающих</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
         <is>
           <t>Сертификат участника</t>
         </is>
@@ -568,18 +542,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2011-07-13</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>13</v>
-      </c>
+          <t>Разметка данных на CVAT для начинающих</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
-        <is>
-          <t>Разметка данных на CVAT для начинающих</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -598,18 +565,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2010-06-21</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>14</v>
-      </c>
+          <t>Разметка данных на CVAT для начинающих</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
-        <is>
-          <t>Разметка данных на CVAT для начинающих</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -628,18 +588,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2013-03-13</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>11</v>
-      </c>
+          <t>Разметка данных на CVAT для начинающих</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
-        <is>
-          <t>Разметка данных на CVAT для начинающих</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -658,18 +611,11 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2010-12-04</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>15</v>
-      </c>
+          <t>Разметка данных на CVAT для начинающих</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
-        <is>
-          <t>Разметка данных на CVAT для начинающих</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
         <is>
           <t> </t>
         </is>

</xml_diff>